<commit_message>
varInfo and createStructure interplay
</commit_message>
<xml_diff>
--- a/tests/testthat/helper_varInfo.xlsx
+++ b/tests/testthat/helper_varInfo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Var.Name</t>
   </si>
@@ -20,6 +20,9 @@
     <t xml:space="preserve">in.DS.und.SH</t>
   </si>
   <si>
+    <t xml:space="preserve">Unterteilung.im.Skalenhandbuch</t>
+  </si>
+  <si>
     <t xml:space="preserve">Layout</t>
   </si>
   <si>
@@ -68,13 +71,16 @@
     <t xml:space="preserve">ja</t>
   </si>
   <si>
+    <t xml:space="preserve">Teil 1a</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">Variable 1</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
+    <t xml:space="preserve">1.01</t>
   </si>
   <si>
     <t xml:space="preserve">nein</t>
@@ -83,13 +89,25 @@
     <t xml:space="preserve">VAR2</t>
   </si>
   <si>
+    <t xml:space="preserve">Teil 1b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Variable 2</t>
   </si>
   <si>
+    <t xml:space="preserve">1.02</t>
+  </si>
+  <si>
     <t xml:space="preserve">VAR3</t>
   </si>
   <si>
+    <t xml:space="preserve">Teil 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Variable 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.01</t>
   </si>
 </sst>
 </file>
@@ -470,155 +488,167 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>